<commit_message>
Added more, expensive items
</commit_message>
<xml_diff>
--- a/Items.xlsx
+++ b/Items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnw\iCloudDrive\Mine\My Programs\CoinGames\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748F7585-2442-462E-AD91-63764AB8D793}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B9EB58-EAF6-4FCB-BA7C-B99153025302}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1272" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{C42CA93E-3A2D-D040-AB9B-E333D2FB9CC9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C42CA93E-3A2D-D040-AB9B-E333D2FB9CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="119">
   <si>
     <t>Name</t>
   </si>
@@ -277,9 +277,6 @@
     <t>Thanos" + apostrophe + "Sword</t>
   </si>
   <si>
-    <t>10^n</t>
-  </si>
-  <si>
     <t>Number in that range</t>
   </si>
   <si>
@@ -316,9 +313,6 @@
     <t>Thanos' Sword</t>
   </si>
   <si>
-    <t>Modulo</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
@@ -335,13 +329,73 @@
   </si>
   <si>
     <t>OP</t>
+  </si>
+  <si>
+    <t>Arc Reactor</t>
+  </si>
+  <si>
+    <t>Kryptonite</t>
+  </si>
+  <si>
+    <t>Air Force One</t>
+  </si>
+  <si>
+    <t>Iron Man Suit</t>
+  </si>
+  <si>
+    <t>Number of digits</t>
+  </si>
+  <si>
+    <t>Klondike Bar</t>
+  </si>
+  <si>
+    <t>Time Machine</t>
+  </si>
+  <si>
+    <t>Bribe</t>
+  </si>
+  <si>
+    <t>Nuclear Fireworks</t>
+  </si>
+  <si>
+    <t>Meme</t>
+  </si>
+  <si>
+    <t>Bigfoot</t>
+  </si>
+  <si>
+    <t>Area 51</t>
+  </si>
+  <si>
+    <t>Loch Ness Monster</t>
+  </si>
+  <si>
+    <t>The Moon</t>
+  </si>
+  <si>
+    <t>A True Cake</t>
+  </si>
+  <si>
+    <t>MissingNo</t>
+  </si>
+  <si>
+    <t>Airpods</t>
+  </si>
+  <si>
+    <t>Ice Cream</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Digits</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -390,13 +444,27 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -436,23 +504,38 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -489,28 +572,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4009156A-C36A-4516-A02C-24F9758B47EE}" name="Table1" displayName="Table1" ref="A1:J63" totalsRowShown="0">
-  <autoFilter ref="A1:J63" xr:uid="{78C1917B-7E31-49F9-99AB-AFB2F1BD8BEA}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I63">
-    <sortCondition descending="1" ref="C1:C63"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4009156A-C36A-4516-A02C-24F9758B47EE}" name="Table1" displayName="Table1" ref="A1:J80" totalsRowShown="0">
+  <autoFilter ref="A1:J80" xr:uid="{78C1917B-7E31-49F9-99AB-AFB2F1BD8BEA}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I80">
+    <sortCondition descending="1" ref="C1:C80"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{B3882E44-A406-45D7-8B81-3BE7D8468DD3}" name="Prefix"/>
-    <tableColumn id="2" xr3:uid="{BBEDCA42-A349-4B8A-B3F6-630CA6A6848E}" name="Name" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{BBEDCA42-A349-4B8A-B3F6-630CA6A6848E}" name="Name" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{EF70BBD7-AFE9-448B-8134-0BE31683DB7F}" name="Cost"/>
     <tableColumn id="4" xr3:uid="{0656EB21-15AB-4A2D-8645-982D7283C115}" name="Column1">
       <calculatedColumnFormula>IF(C2&gt;2147483647,"L","")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{72E00DC1-7F07-4212-9067-1519DBF1E8CB}" name="Boost"/>
-    <tableColumn id="6" xr3:uid="{4C3041D4-FCB0-4127-ACBC-989B299F0011}" name="Quantity" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{F74CFCBD-6EB6-4116-8F58-FAA3BD72544B}" name="Final">
-      <calculatedColumnFormula>IF(A2="",_xlfn.CONCAT($K$1,$K$2,B2,$K$2,$K$3,C2,D2,$K$3,E2,$K$3,F2,"),",),_xlfn.CONCAT($K$1,$K$2,A2,$K$2,$K$3,$K$2,B2,$K$2,$K$3,C2,D2,$K$3,E2,$K$3,F2,"),"))</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{4C3041D4-FCB0-4127-ACBC-989B299F0011}" name="Quantity" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{F74CFCBD-6EB6-4116-8F58-FAA3BD72544B}" name="Final" dataDxfId="3">
+      <calculatedColumnFormula>_xlfn.CONCAT($K$1,$K$3,B2,$K$3,$K$2,C2,D2,$K$2,E2,$K$2,F2,"),")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{ED093BC7-1767-47E6-9724-AAE846529AF1}" name="Messages needed to earn back the amount of coins spend" dataDxfId="1">
+    <tableColumn id="8" xr3:uid="{ED093BC7-1767-47E6-9724-AAE846529AF1}" name="Messages needed to earn back the amount of coins spend" dataDxfId="2">
       <calculatedColumnFormula>C2/E2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{CED6810C-AE22-4E72-BAF9-196C471149E4}" name="Modulo" dataDxfId="0">
-      <calculatedColumnFormula>FLOOR(LOG10(C2),1)</calculatedColumnFormula>
+    <tableColumn id="9" xr3:uid="{CED6810C-AE22-4E72-BAF9-196C471149E4}" name="Digits" dataDxfId="0">
+      <calculatedColumnFormula>CEILING(LOG10(C2),1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{4B948BE7-CCBA-44E6-88FF-EF66EE6101A1}" name="Egg"/>
   </tableColumns>
@@ -2617,19 +2700,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6AE1024-0C54-6843-8563-9D359055A938}">
-  <dimension ref="A1:N63"/>
+  <dimension ref="A1:N92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="3" max="3" width="11.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="11.19921875" customWidth="1"/>
+    <col min="5" max="5" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.19921875" customWidth="1"/>
     <col min="8" max="8" width="51.296875" customWidth="1"/>
-    <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="11.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -2643,7 +2727,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -2655,22 +2739,22 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J1" t="s">
         <v>94</v>
-      </c>
-      <c r="J1" t="s">
-        <v>96</v>
       </c>
       <c r="K1" t="s">
         <v>78</v>
       </c>
       <c r="M1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N1" t="s">
         <v>81</v>
-      </c>
-      <c r="N1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -2690,17 +2774,17 @@
       <c r="F2" s="2">
         <v>1</v>
       </c>
-      <c r="G2" t="e">
-        <f>IF(A2="",_xlfn.CONCAT($K$1,#REF!,B2,#REF!,$K$2,C2,D2,$K$2,E2,$K$2,F2,"),",),_xlfn.CONCAT($K$1,#REF!,A2,#REF!,$K$2,#REF!,B2,#REF!,$K$2,C2,D2,$K$2,E2,$K$2,F2,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H2" s="12">
-        <f t="shared" ref="H2:H30" si="1">C2/E2</f>
+      <c r="G2" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B2,$K$3,$K$2,C2,D2,$K$2,E2,$K$2,F2,"),")</f>
+        <v>new Upgrade("International Space Station",50400000000L,196199000,1),</v>
+      </c>
+      <c r="H2" s="11">
+        <f t="shared" ref="H2:H9" si="1">C2/E2</f>
         <v>256.88204323161688</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I30" si="2">FLOOR(LOG10(C2),1)</f>
-        <v>10</v>
+        <f t="shared" ref="I2:I33" si="2">CEILING(LOG10(C2),1)</f>
+        <v>11</v>
       </c>
       <c r="K2" t="s">
         <v>77</v>
@@ -2710,7 +2794,7 @@
       </c>
       <c r="N2" s="4">
         <f>COUNTIF(I:I,M2)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -2730,24 +2814,27 @@
       <c r="F3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" t="e">
-        <f>IF(A3="",_xlfn.CONCAT($K$1,#REF!,B3,#REF!,$K$2,C3,D3,$K$2,E3,$K$2,F3,"),",),_xlfn.CONCAT($K$1,#REF!,A3,#REF!,$K$2,#REF!,B3,#REF!,$K$2,C3,D3,$K$2,E3,$K$2,F3,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H3" s="12">
+      <c r="G3" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B3,$K$3,$K$2,C3,D3,$K$2,E3,$K$2,F3,"),")</f>
+        <v>new Upgrade("Diamond Armor",5307786900L,25100000,1),</v>
+      </c>
+      <c r="H3" s="11">
         <f t="shared" si="1"/>
         <v>211.46561354581672</v>
       </c>
       <c r="I3">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="K3" t="s">
+        <v>76</v>
       </c>
       <c r="M3" s="3">
         <v>2</v>
       </c>
       <c r="N3" s="4">
         <f>COUNTIF(I:I,M3)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -2767,17 +2854,17 @@
       <c r="F4" s="2">
         <v>1</v>
       </c>
-      <c r="G4" t="e">
-        <f>IF(A4="",_xlfn.CONCAT($K$1,#REF!,B4,#REF!,$K$2,C4,D4,$K$2,E4,$K$2,F4,"),",),_xlfn.CONCAT($K$1,#REF!,A4,#REF!,$K$2,#REF!,B4,#REF!,$K$2,C4,D4,$K$2,E4,$K$2,F4,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H4" s="12">
+      <c r="G4" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B4,$K$3,$K$2,C4,D4,$K$2,E4,$K$2,F4,"),")</f>
+        <v>new Upgrade("Hubble Telescope",2870000000L,14320231,1),</v>
+      </c>
+      <c r="H4" s="11">
         <f t="shared" si="1"/>
         <v>200.41576144965819</v>
       </c>
       <c r="I4">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M4" s="3">
         <v>3</v>
@@ -2804,24 +2891,29 @@
       <c r="F5" s="2">
         <v>1</v>
       </c>
-      <c r="G5" t="e">
-        <f>IF(A5="",_xlfn.CONCAT($K$1,#REF!,B5,#REF!,$K$2,C5,D5,$K$2,E5,$K$2,F5,"),",),_xlfn.CONCAT($K$1,#REF!,A5,#REF!,$K$2,#REF!,B5,#REF!,$K$2,C5,D5,$K$2,E5,$K$2,F5,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H5" s="12">
+      <c r="G5" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B5,$K$3,$K$2,C5,D5,$K$2,E5,$K$2,F5,"),")</f>
+        <v>new Upgrade("Baby Shark",2639860696L,13199303,1),</v>
+      </c>
+      <c r="H5" s="11">
         <f t="shared" si="1"/>
         <v>200.00000727311132</v>
       </c>
       <c r="I5">
         <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="K5" s="13" t="str">
+        <f>_xlfn.CONCAT(G2:G5000)</f>
+        <v>new Upgrade("International Space Station",50400000000L,196199000,1),new Upgrade("Diamond Armor",5307786900L,25100000,1),new Upgrade("Hubble Telescope",2870000000L,14320231,1),new Upgrade("Baby Shark",2639860696L,13199303,1),new Upgrade("Infinity Gauntlet",2147483647,13166600,1),new Upgrade("Wayne Manor",800000000,3970009,1),new Upgrade("Because I'm Batman!",682450750,3402000,1),new Upgrade("141-year-old newspaper",230000000,948324,1),new Upgrade("1963 Ferrari GTO",52000000,196300,5),new Upgrade("Honus Wagner Rookie Card",2000000,8727,3),new Upgrade("Captain America's Shield",17871941,113100,1),new Upgrade("Gold Plated Bugatti Veyron",10004738,43253,1),new Upgrade("Mjolnir",4490000,30000,1),new Upgrade("Crystal Piano",3200000,14324,1),new Upgrade("Thanos' Sword",2014000,10115,1),new Upgrade("The Tumbler Batmobile",1800000,6930,1),new Upgrade("Magnetic Floating Bed",1600000,8000,1),new Upgrade("All of the Pokemon",1510000,8090,1),new Upgrade("Ferrari Enzo",1325000,5500,7),new Upgrade("The Ultimate Ultimate Weapon",1230000,4920,6),new Upgrade("Darth Vader's Helmet",1138000,7486,1),new Upgrade("Crisp $1,000,000 bill",999999,0,100),new Upgrade("Tank",858000,3750,10),new Upgrade("Lightsaber",300000,1977,6),new Upgrade("Pet Dragon",630000,3030,5),new Upgrade("Smash Ball",400000,1500,6),new Upgrade("Legolas's Bow",301800,2110,1),new Upgrade("Phaser Rifle",200000,1000,1),new Upgrade("Six-Shooter",130364,600,6),new Upgrade("Kylo Ren's Helmet",200000,1350,1),new Upgrade("Nuclear Bomb",500235,2390,5),new Upgrade("Bowcaster",155893,563,10),new Upgrade("Genesis Device",765482,4570,1),new Upgrade("A bad feeling about this",166830,1138,1),new Upgrade("Death Star",1344339,7324,2),new Upgrade("Rocket",100000,500,10),new Upgrade("Ring of Power",2963500,19776,19),new Upgrade("Stormbreaker",1375947,10000,1),new Upgrade("Medpack",100000,500,10),new Upgrade("Mario's Hat",1019358,5342,1),new Upgrade("Blender (the program)",530000,2140,10),new Upgrade("iPhone XR",300000,1215,1),new Upgrade("Stormtrooper Helmet",13630,70,10),new Upgrade("Sandwitch",22414,84,10),new Upgrade("Oculus",39999,199,10),new Upgrade("Shards of Narsil",20000,97,6),new Upgrade("Batarang",14645,70,10),new Upgrade("Sword",10000,51,100),new Upgrade("Water Bottle",10000,49,10),new Upgrade("Easy Button",667186,2839,10),new Upgrade("Blender (for food)",10000,43,7),new Upgrade("The Piece of Resistance",998520,4950,1),new Upgrade("Shield",5000,25,200),new Upgrade("Shark Repellent Bat Spray",1996,10,4),new Upgrade("Kirk's Glasses",957440,4329,1),new Upgrade("Popcorn",1000,5,100),new Upgrade("Book",451,2,10),new Upgrade("Cookie",100,3,1),new Upgrade("Lego Brick",200,1,100),new Upgrade("Bug",1,-1,128),new Upgrade("Arc Reactor",59637044043L,141467051,1),new Upgrade("Kryptonite",2110089696934650L,4096534023712,1),new Upgrade("Air Force One",83250280290413900L,151941677102307,1),new Upgrade("Cheat",1,1,1),new Upgrade("Ice Cream",40896568606L,97793577,),new Upgrade("Klondike Bar",4275149189933540000L,7331994574249420,1),new Upgrade("Time Machine",83745097494464L,172216610960,1),new Upgrade("Bribe",1000000,0,1),new Upgrade("Nuclear Fireworks",81247450573750L,167173305334,1),new Upgrade("Meme",1755841378694L,3886619829,1),new Upgrade("Bigfoot",79837291968785L,164324651505,1),new Upgrade("Area 51",5704058330541L,12338782071,1),new Upgrade("Loch Ness Monster",2221819257185L,4895303336,1),new Upgrade("The Moon",839548670437L,1885876413,1),new Upgrade("A True Cake",1248529473245030L,2446152366149,5),new Upgrade("MissingNo",55905021527L,132795976,1),new Upgrade("Airpods",37910263806L,90799614,2),new Upgrade("Iron Man Suit",1858055186797720L,3615205690620,2),new Upgrade("Debug Byte",1,0,256),</v>
+      </c>
+      <c r="L5" s="13"/>
       <c r="M5" s="3">
         <v>4</v>
       </c>
       <c r="N5" s="4">
         <f>COUNTIF(I:I,M5)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="6" customFormat="1">
@@ -2841,24 +2933,26 @@
       <c r="F6" s="9">
         <v>1</v>
       </c>
-      <c r="G6" s="6" t="e">
-        <f>IF(A6="",_xlfn.CONCAT($K$1,#REF!,B6,#REF!,$K$2,C6,D6,$K$2,E6,$K$2,F6,"),",),_xlfn.CONCAT($K$1,#REF!,A6,#REF!,$K$2,#REF!,B6,#REF!,$K$2,C6,D6,$K$2,E6,$K$2,F6,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H6" s="13">
+      <c r="G6" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B6,$K$3,$K$2,C6,D6,$K$2,E6,$K$2,F6,"),")</f>
+        <v>new Upgrade("Infinity Gauntlet",2147483647,13166600,1),</v>
+      </c>
+      <c r="H6" s="12">
         <f t="shared" si="1"/>
         <v>163.10084964987163</v>
       </c>
       <c r="I6" s="6">
         <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
       <c r="M6" s="10">
         <v>5</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6" s="4">
         <f>COUNTIF(I:I,M6)</f>
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -2878,29 +2972,31 @@
       <c r="F7" s="2">
         <v>1</v>
       </c>
-      <c r="G7" t="e">
-        <f>IF(A7="",_xlfn.CONCAT($K$1,#REF!,B7,#REF!,$K$2,C7,D7,$K$2,E7,$K$2,F7,"),",),_xlfn.CONCAT($K$1,#REF!,A7,#REF!,$K$2,#REF!,B7,#REF!,$K$2,C7,D7,$K$2,E7,$K$2,F7,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H7" s="12">
+      <c r="G7" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B7,$K$3,$K$2,C7,D7,$K$2,E7,$K$2,F7,"),")</f>
+        <v>new Upgrade("Wayne Manor",800000000,3970009,1),</v>
+      </c>
+      <c r="H7" s="11">
         <f t="shared" si="1"/>
         <v>201.51087818692602</v>
       </c>
       <c r="I7">
         <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
       <c r="M7" s="3">
         <v>6</v>
       </c>
       <c r="N7" s="4">
         <f>COUNTIF(I:I,M7)</f>
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="B8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8">
         <v>682450750</v>
@@ -2915,24 +3011,24 @@
       <c r="F8" s="2">
         <v>1</v>
       </c>
-      <c r="G8" t="e">
-        <f>IF(A8="",_xlfn.CONCAT($K$1,#REF!,B8,#REF!,$K$2,C8,D8,$K$2,E8,$K$2,F8,"),",),_xlfn.CONCAT($K$1,#REF!,A8,#REF!,$K$2,#REF!,B8,#REF!,$K$2,C8,D8,$K$2,E8,$K$2,F8,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H8" s="12">
+      <c r="G8" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B8,$K$3,$K$2,C8,D8,$K$2,E8,$K$2,F8,"),")</f>
+        <v>new Upgrade("Because I'm Batman!",682450750,3402000,1),</v>
+      </c>
+      <c r="H8" s="11">
         <f t="shared" si="1"/>
         <v>200.60280717225163</v>
       </c>
       <c r="I8">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M8" s="5">
         <v>7</v>
       </c>
       <c r="N8" s="4">
         <f>COUNTIF(I:I,M8)</f>
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -2952,17 +3048,17 @@
       <c r="F9" s="2">
         <v>1</v>
       </c>
-      <c r="G9" t="e">
-        <f>IF(A9="",_xlfn.CONCAT($K$1,#REF!,B9,#REF!,$K$2,C9,D9,$K$2,E9,$K$2,F9,"),",),_xlfn.CONCAT($K$1,#REF!,A9,#REF!,$K$2,#REF!,B9,#REF!,$K$2,C9,D9,$K$2,E9,$K$2,F9,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H9" s="12">
+      <c r="G9" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B9,$K$3,$K$2,C9,D9,$K$2,E9,$K$2,F9,"),")</f>
+        <v>new Upgrade("141-year-old newspaper",230000000,948324,1),</v>
+      </c>
+      <c r="H9" s="11">
         <f t="shared" si="1"/>
         <v>242.53314268119334</v>
       </c>
       <c r="I9">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M9" s="3">
         <v>8</v>
@@ -2989,24 +3085,24 @@
       <c r="F10" s="2">
         <v>5</v>
       </c>
-      <c r="G10" t="e">
-        <f>IF(A10="",_xlfn.CONCAT($K$1,#REF!,B10,#REF!,$K$2,C10,D10,$K$2,E10,$K$2,F10,"),",),_xlfn.CONCAT($K$1,#REF!,A10,#REF!,$K$2,#REF!,B10,#REF!,$K$2,C10,D10,$K$2,E10,$K$2,F10,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H10" s="12">
-        <f t="shared" si="1"/>
+      <c r="G10" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B10,$K$3,$K$2,C10,D10,$K$2,E10,$K$2,F10,"),")</f>
+        <v>new Upgrade("1963 Ferrari GTO",52000000,196300,5),</v>
+      </c>
+      <c r="H10" s="11">
+        <f>C10/E10</f>
         <v>264.9006622516556</v>
       </c>
       <c r="I10">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M10" s="3">
         <v>9</v>
       </c>
       <c r="N10" s="4">
         <f>COUNTIF(I:I,M10)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -3027,29 +3123,29 @@
       <c r="F11" s="2">
         <v>3</v>
       </c>
-      <c r="G11" t="e">
-        <f>IF(A11="",_xlfn.CONCAT($K$1,#REF!,B11,#REF!,$K$2,C11,D11,$K$2,E11,$K$2,F11,"),",),_xlfn.CONCAT($K$1,#REF!,A11,#REF!,$K$2,#REF!,B11,#REF!,$K$2,C11,D11,$K$2,E11,$K$2,F11,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H11" s="12">
-        <f t="shared" si="1"/>
+      <c r="G11" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B11,$K$3,$K$2,C11,D11,$K$2,E11,$K$2,F11,"),")</f>
+        <v>new Upgrade("Honus Wagner Rookie Card",2000000,8727,3),</v>
+      </c>
+      <c r="H11" s="11">
+        <f>C11/E11</f>
         <v>229.17382834880257</v>
       </c>
       <c r="I11">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M11" s="3">
         <v>10</v>
       </c>
       <c r="N11" s="4">
         <f>COUNTIF(I:I,M11)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="6" customFormat="1">
       <c r="B12" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" s="6">
         <v>17871941</v>
@@ -3064,24 +3160,24 @@
       <c r="F12" s="9">
         <v>1</v>
       </c>
-      <c r="G12" s="6" t="e">
-        <f>IF(A12="",_xlfn.CONCAT($K$1,#REF!,B12,#REF!,$K$2,C12,D12,$K$2,E12,$K$2,F12,"),",),_xlfn.CONCAT($K$1,#REF!,A12,#REF!,$K$2,#REF!,B12,#REF!,$K$2,C12,D12,$K$2,E12,$K$2,F12,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H12" s="13">
-        <f t="shared" si="1"/>
+      <c r="G12" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B12,$K$3,$K$2,C12,D12,$K$2,E12,$K$2,F12,"),")</f>
+        <v>new Upgrade("Captain America's Shield",17871941,113100,1),</v>
+      </c>
+      <c r="H12" s="12">
+        <f>C12/E12</f>
         <v>158.01893015030947</v>
       </c>
       <c r="I12" s="6">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M12" s="10">
         <v>11</v>
       </c>
-      <c r="N12" s="11">
+      <c r="N12" s="4">
         <f>COUNTIF(I:I,M12)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -3101,24 +3197,24 @@
       <c r="F13" s="2">
         <v>1</v>
       </c>
-      <c r="G13" t="e">
-        <f>IF(A13="",_xlfn.CONCAT($K$1,#REF!,B13,#REF!,$K$2,C13,D13,$K$2,E13,$K$2,F13,"),",),_xlfn.CONCAT($K$1,#REF!,A13,#REF!,$K$2,#REF!,B13,#REF!,$K$2,C13,D13,$K$2,E13,$K$2,F13,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H13" s="12">
-        <f t="shared" si="1"/>
+      <c r="G13" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B13,$K$3,$K$2,C13,D13,$K$2,E13,$K$2,F13,"),")</f>
+        <v>new Upgrade("Gold Plated Bugatti Veyron",10004738,43253,1),</v>
+      </c>
+      <c r="H13" s="11">
+        <f>C13/E13</f>
         <v>231.30737752294638</v>
       </c>
       <c r="I13">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M13" s="3">
         <v>13</v>
       </c>
       <c r="N13" s="4">
         <f>COUNTIF(I:I,M13)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="6" customFormat="1">
@@ -3138,24 +3234,24 @@
       <c r="F14" s="9">
         <v>1</v>
       </c>
-      <c r="G14" s="6" t="e">
-        <f>IF(A14="",_xlfn.CONCAT($K$1,#REF!,B14,#REF!,$K$2,C14,D14,$K$2,E14,$K$2,F14,"),",),_xlfn.CONCAT($K$1,#REF!,A14,#REF!,$K$2,#REF!,B14,#REF!,$K$2,C14,D14,$K$2,E14,$K$2,F14,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H14" s="13">
-        <f t="shared" si="1"/>
+      <c r="G14" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B14,$K$3,$K$2,C14,D14,$K$2,E14,$K$2,F14,"),")</f>
+        <v>new Upgrade("Mjolnir",4490000,30000,1),</v>
+      </c>
+      <c r="H14" s="12">
+        <f>C14/E14</f>
         <v>149.66666666666666</v>
       </c>
       <c r="I14" s="6">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M14" s="10">
         <v>14</v>
       </c>
-      <c r="N14" s="11">
+      <c r="N14" s="4">
         <f>COUNTIF(I:I,M14)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -3175,17 +3271,17 @@
       <c r="F15" s="2">
         <v>1</v>
       </c>
-      <c r="G15" t="e">
-        <f>IF(A15="",_xlfn.CONCAT($K$1,#REF!,B15,#REF!,$K$2,C15,D15,$K$2,E15,$K$2,F15,"),",),_xlfn.CONCAT($K$1,#REF!,A15,#REF!,$K$2,#REF!,B15,#REF!,$K$2,C15,D15,$K$2,E15,$K$2,F15,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H15" s="12">
-        <f t="shared" si="1"/>
+      <c r="G15" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B15,$K$3,$K$2,C15,D15,$K$2,E15,$K$2,F15,"),")</f>
+        <v>new Upgrade("Crystal Piano",3200000,14324,1),</v>
+      </c>
+      <c r="H15" s="11">
+        <f>C15/E15</f>
         <v>223.40128455738619</v>
       </c>
       <c r="I15">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M15" s="3">
         <v>15</v>
@@ -3197,7 +3293,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="B16" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16">
         <v>2014000</v>
@@ -3213,24 +3309,24 @@
       <c r="F16" s="2">
         <v>1</v>
       </c>
-      <c r="G16" t="e">
-        <f>IF(A16="",_xlfn.CONCAT($K$1,#REF!,B16,#REF!,$K$2,C16,D16,$K$2,E16,$K$2,F16,"),",),_xlfn.CONCAT($K$1,#REF!,A16,#REF!,$K$2,#REF!,B16,#REF!,$K$2,C16,D16,$K$2,E16,$K$2,F16,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H16" s="12">
-        <f t="shared" si="1"/>
+      <c r="G16" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B16,$K$3,$K$2,C16,D16,$K$2,E16,$K$2,F16,"),")</f>
+        <v>new Upgrade("Thanos' Sword",2014000,10115,1),</v>
+      </c>
+      <c r="H16" s="11">
+        <f>C16/E16</f>
         <v>199.11023232822541</v>
       </c>
       <c r="I16">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M16" s="3">
         <v>16</v>
       </c>
       <c r="N16" s="4">
         <f>COUNTIF(I:I,M16)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:14">
@@ -3250,24 +3346,24 @@
       <c r="F17" s="2">
         <v>1</v>
       </c>
-      <c r="G17" t="e">
-        <f>IF(A17="",_xlfn.CONCAT($K$1,#REF!,B17,#REF!,$K$2,C17,D17,$K$2,E17,$K$2,F17,"),",),_xlfn.CONCAT($K$1,#REF!,A17,#REF!,$K$2,#REF!,B17,#REF!,$K$2,C17,D17,$K$2,E17,$K$2,F17,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H17" s="12">
-        <f t="shared" si="1"/>
+      <c r="G17" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B17,$K$3,$K$2,C17,D17,$K$2,E17,$K$2,F17,"),")</f>
+        <v>new Upgrade("The Tumbler Batmobile",1800000,6930,1),</v>
+      </c>
+      <c r="H17" s="11">
+        <f>C17/E17</f>
         <v>259.74025974025972</v>
       </c>
       <c r="I17">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M17" s="3">
         <v>17</v>
       </c>
       <c r="N17" s="4">
         <f>COUNTIF(I:I,M17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:14">
@@ -3287,17 +3383,17 @@
       <c r="F18" s="2">
         <v>1</v>
       </c>
-      <c r="G18" t="e">
-        <f>IF(A18="",_xlfn.CONCAT($K$1,#REF!,B18,#REF!,$K$2,C18,D18,$K$2,E18,$K$2,F18,"),",),_xlfn.CONCAT($K$1,#REF!,A18,#REF!,$K$2,#REF!,B18,#REF!,$K$2,C18,D18,$K$2,E18,$K$2,F18,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H18" s="12">
-        <f t="shared" si="1"/>
+      <c r="G18" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B18,$K$3,$K$2,C18,D18,$K$2,E18,$K$2,F18,"),")</f>
+        <v>new Upgrade("Magnetic Floating Bed",1600000,8000,1),</v>
+      </c>
+      <c r="H18" s="11">
+        <f>C18/E18</f>
         <v>200</v>
       </c>
       <c r="I18">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M18" s="3">
         <v>18</v>
@@ -3324,24 +3420,24 @@
       <c r="F19" s="2">
         <v>1</v>
       </c>
-      <c r="G19" t="e">
-        <f>IF(A19="",_xlfn.CONCAT($K$1,#REF!,B19,#REF!,$K$2,C19,D19,$K$2,E19,$K$2,F19,"),",),_xlfn.CONCAT($K$1,#REF!,A19,#REF!,$K$2,#REF!,B19,#REF!,$K$2,C19,D19,$K$2,E19,$K$2,F19,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H19" s="12">
-        <f t="shared" si="1"/>
+      <c r="G19" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B19,$K$3,$K$2,C19,D19,$K$2,E19,$K$2,F19,"),")</f>
+        <v>new Upgrade("All of the Pokemon",1510000,8090,1),</v>
+      </c>
+      <c r="H19" s="11">
+        <f>C19/E19</f>
         <v>186.65018541409148</v>
       </c>
       <c r="I19">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M19" s="3">
         <v>19</v>
       </c>
       <c r="N19" s="4">
         <f>COUNTIF(I:I,M19)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:14">
@@ -3361,17 +3457,17 @@
       <c r="F20" s="2">
         <v>7</v>
       </c>
-      <c r="G20" t="e">
-        <f>IF(A20="",_xlfn.CONCAT($K$1,#REF!,B20,#REF!,$K$2,C20,D20,$K$2,E20,$K$2,F20,"),",),_xlfn.CONCAT($K$1,#REF!,A20,#REF!,$K$2,#REF!,B20,#REF!,$K$2,C20,D20,$K$2,E20,$K$2,F20,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H20" s="12">
-        <f t="shared" si="1"/>
+      <c r="G20" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B20,$K$3,$K$2,C20,D20,$K$2,E20,$K$2,F20,"),")</f>
+        <v>new Upgrade("Ferrari Enzo",1325000,5500,7),</v>
+      </c>
+      <c r="H20" s="11">
+        <f>C20/E20</f>
         <v>240.90909090909091</v>
       </c>
       <c r="I20">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M20" s="3">
         <v>20</v>
@@ -3399,22 +3495,23 @@
       <c r="F21" s="2">
         <v>6</v>
       </c>
-      <c r="G21" t="e">
-        <f>IF(A21="",_xlfn.CONCAT($K$1,#REF!,B21,#REF!,$K$2,C21,D21,$K$2,E21,$K$2,F21,"),",),_xlfn.CONCAT($K$1,#REF!,A21,#REF!,$K$2,#REF!,B21,#REF!,$K$2,C21,D21,$K$2,E21,$K$2,F21,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H21" s="12">
-        <f t="shared" si="1"/>
+      <c r="G21" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B21,$K$3,$K$2,C21,D21,$K$2,E21,$K$2,F21,"),")</f>
+        <v>new Upgrade("The Ultimate Ultimate Weapon",1230000,4920,6),</v>
+      </c>
+      <c r="H21" s="11">
+        <f>C21/E21</f>
         <v>250</v>
       </c>
       <c r="I21">
         <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="N21" s="4"/>
     </row>
     <row r="22" spans="2:14" s="6" customFormat="1">
       <c r="B22" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C22" s="6">
         <v>1138000</v>
@@ -3429,18 +3526,19 @@
       <c r="F22" s="9">
         <v>1</v>
       </c>
-      <c r="G22" s="6" t="e">
-        <f>IF(A22="",_xlfn.CONCAT($K$1,#REF!,B22,#REF!,$K$2,C22,D22,$K$2,E22,$K$2,F22,"),",),_xlfn.CONCAT($K$1,#REF!,A22,#REF!,$K$2,#REF!,B22,#REF!,$K$2,C22,D22,$K$2,E22,$K$2,F22,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H22" s="13">
-        <f t="shared" si="1"/>
+      <c r="G22" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B22,$K$3,$K$2,C22,D22,$K$2,E22,$K$2,F22,"),")</f>
+        <v>new Upgrade("Darth Vader's Helmet",1138000,7486,1),</v>
+      </c>
+      <c r="H22" s="12">
+        <f>C22/E22</f>
         <v>152.0170985840235</v>
       </c>
       <c r="I22" s="6">
         <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="N22" s="4"/>
     </row>
     <row r="23" spans="2:14">
       <c r="B23" s="1" t="s">
@@ -3459,18 +3557,19 @@
       <c r="F23" s="2">
         <v>100</v>
       </c>
-      <c r="G23" t="e">
-        <f>IF(A23="",_xlfn.CONCAT($K$1,#REF!,B23,#REF!,$K$2,C23,D23,$K$2,E23,$K$2,F23,"),",),_xlfn.CONCAT($K$1,#REF!,A23,#REF!,$K$2,#REF!,B23,#REF!,$K$2,C23,D23,$K$2,E23,$K$2,F23,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H23" s="12" t="e">
-        <f t="shared" si="1"/>
+      <c r="G23" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B23,$K$3,$K$2,C23,D23,$K$2,E23,$K$2,F23,"),")</f>
+        <v>new Upgrade("Crisp $1,000,000 bill",999999,0,100),</v>
+      </c>
+      <c r="H23" s="11" t="e">
+        <f>C23/E23</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I23">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="N23" s="4"/>
     </row>
     <row r="24" spans="2:14">
       <c r="B24" s="1" t="s">
@@ -3490,18 +3589,19 @@
       <c r="F24" s="2">
         <v>10</v>
       </c>
-      <c r="G24" t="e">
-        <f>IF(A24="",_xlfn.CONCAT($K$1,#REF!,B24,#REF!,$K$2,C24,D24,$K$2,E24,$K$2,F24,"),",),_xlfn.CONCAT($K$1,#REF!,A24,#REF!,$K$2,#REF!,B24,#REF!,$K$2,C24,D24,$K$2,E24,$K$2,F24,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H24" s="12">
-        <f t="shared" si="1"/>
+      <c r="G24" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B24,$K$3,$K$2,C24,D24,$K$2,E24,$K$2,F24,"),")</f>
+        <v>new Upgrade("Tank",858000,3750,10),</v>
+      </c>
+      <c r="H24" s="11">
+        <f>C24/E24</f>
         <v>228.8</v>
       </c>
       <c r="I24">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="N24" s="4"/>
     </row>
     <row r="25" spans="2:14" s="6" customFormat="1">
       <c r="B25" s="7" t="s">
@@ -3520,18 +3620,19 @@
       <c r="F25" s="9">
         <v>6</v>
       </c>
-      <c r="G25" s="6" t="e">
-        <f>IF(A25="",_xlfn.CONCAT($K$1,#REF!,B25,#REF!,$K$2,C25,D25,$K$2,E25,$K$2,F25,"),",),_xlfn.CONCAT($K$1,#REF!,A25,#REF!,$K$2,#REF!,B25,#REF!,$K$2,C25,D25,$K$2,E25,$K$2,F25,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H25" s="13">
-        <f t="shared" si="1"/>
+      <c r="G25" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B25,$K$3,$K$2,C25,D25,$K$2,E25,$K$2,F25,"),")</f>
+        <v>new Upgrade("Lightsaber",300000,1977,6),</v>
+      </c>
+      <c r="H25" s="12">
+        <f>C25/E25</f>
         <v>151.74506828528072</v>
       </c>
       <c r="I25" s="6">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="N25" s="4"/>
     </row>
     <row r="26" spans="2:14">
       <c r="B26" s="1" t="s">
@@ -3550,18 +3651,19 @@
       <c r="F26" s="2">
         <v>5</v>
       </c>
-      <c r="G26" t="e">
-        <f>IF(A26="",_xlfn.CONCAT($K$1,#REF!,B26,#REF!,$K$2,C26,D26,$K$2,E26,$K$2,F26,"),",),_xlfn.CONCAT($K$1,#REF!,A26,#REF!,$K$2,#REF!,B26,#REF!,$K$2,C26,D26,$K$2,E26,$K$2,F26,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H26" s="12">
-        <f t="shared" si="1"/>
+      <c r="G26" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B26,$K$3,$K$2,C26,D26,$K$2,E26,$K$2,F26,"),")</f>
+        <v>new Upgrade("Pet Dragon",630000,3030,5),</v>
+      </c>
+      <c r="H26" s="11">
+        <f>C26/E26</f>
         <v>207.92079207920793</v>
       </c>
       <c r="I26">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="N26" s="4"/>
     </row>
     <row r="27" spans="2:14">
       <c r="B27" s="1" t="s">
@@ -3581,22 +3683,23 @@
       <c r="F27" s="2">
         <v>6</v>
       </c>
-      <c r="G27" t="e">
-        <f>IF(A27="",_xlfn.CONCAT($K$1,#REF!,B27,#REF!,$K$2,C27,D27,$K$2,E27,$K$2,F27,"),",),_xlfn.CONCAT($K$1,#REF!,A27,#REF!,$K$2,#REF!,B27,#REF!,$K$2,C27,D27,$K$2,E27,$K$2,F27,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H27" s="12">
-        <f t="shared" si="1"/>
+      <c r="G27" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B27,$K$3,$K$2,C27,D27,$K$2,E27,$K$2,F27,"),")</f>
+        <v>new Upgrade("Smash Ball",400000,1500,6),</v>
+      </c>
+      <c r="H27" s="11">
+        <f>C27/E27</f>
         <v>266.66666666666669</v>
       </c>
       <c r="I27">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="N27" s="4"/>
     </row>
     <row r="28" spans="2:14" s="6" customFormat="1">
       <c r="B28" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C28" s="6">
         <v>301800</v>
@@ -3611,18 +3714,19 @@
       <c r="F28" s="9">
         <v>1</v>
       </c>
-      <c r="G28" s="6" t="e">
-        <f>IF(A28="",_xlfn.CONCAT($K$1,#REF!,B28,#REF!,$K$2,C28,D28,$K$2,E28,$K$2,F28,"),",),_xlfn.CONCAT($K$1,#REF!,A28,#REF!,$K$2,#REF!,B28,#REF!,$K$2,C28,D28,$K$2,E28,$K$2,F28,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H28" s="13">
-        <f t="shared" si="1"/>
+      <c r="G28" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B28,$K$3,$K$2,C28,D28,$K$2,E28,$K$2,F28,"),")</f>
+        <v>new Upgrade("Legolas's Bow",301800,2110,1),</v>
+      </c>
+      <c r="H28" s="12">
+        <f>C28/E28</f>
         <v>143.03317535545023</v>
       </c>
       <c r="I28" s="6">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="N28" s="4"/>
     </row>
     <row r="29" spans="2:14">
       <c r="B29" s="1" t="s">
@@ -3641,18 +3745,19 @@
       <c r="F29" s="2">
         <v>1</v>
       </c>
-      <c r="G29" t="e">
-        <f>IF(A29="",_xlfn.CONCAT($K$1,#REF!,B29,#REF!,$K$2,C29,D29,$K$2,E29,$K$2,F29,"),",),_xlfn.CONCAT($K$1,#REF!,A29,#REF!,$K$2,#REF!,B29,#REF!,$K$2,C29,D29,$K$2,E29,$K$2,F29,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H29" s="12">
-        <f t="shared" si="1"/>
+      <c r="G29" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B29,$K$3,$K$2,C29,D29,$K$2,E29,$K$2,F29,"),")</f>
+        <v>new Upgrade("Phaser Rifle",200000,1000,1),</v>
+      </c>
+      <c r="H29" s="11">
+        <f>C29/E29</f>
         <v>200</v>
       </c>
       <c r="I29">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="N29" s="4"/>
     </row>
     <row r="30" spans="2:14">
       <c r="B30" s="1" t="s">
@@ -3671,22 +3776,23 @@
       <c r="F30" s="2">
         <v>6</v>
       </c>
-      <c r="G30" t="e">
-        <f>IF(A30="",_xlfn.CONCAT($K$1,#REF!,B30,#REF!,$K$2,C30,D30,$K$2,E30,$K$2,F30,"),",),_xlfn.CONCAT($K$1,#REF!,A30,#REF!,$K$2,#REF!,B30,#REF!,$K$2,C30,D30,$K$2,E30,$K$2,F30,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H30" s="12">
-        <f t="shared" si="1"/>
+      <c r="G30" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B30,$K$3,$K$2,C30,D30,$K$2,E30,$K$2,F30,"),")</f>
+        <v>new Upgrade("Six-Shooter",130364,600,6),</v>
+      </c>
+      <c r="H30" s="11">
+        <f>C30/E30</f>
         <v>217.27333333333334</v>
       </c>
       <c r="I30">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="N30" s="4"/>
     </row>
     <row r="31" spans="2:14" s="6" customFormat="1">
       <c r="B31" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C31" s="6">
         <v>200000</v>
@@ -3701,18 +3807,19 @@
       <c r="F31" s="9">
         <v>1</v>
       </c>
-      <c r="G31" s="6" t="e">
-        <f>IF(A31="",_xlfn.CONCAT($K$1,#REF!,B31,#REF!,$K$2,C31,D31,$K$2,E31,$K$2,F31,"),",),_xlfn.CONCAT($K$1,#REF!,A31,#REF!,$K$2,#REF!,B31,#REF!,$K$2,C31,D31,$K$2,E31,$K$2,F31,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H31" s="13">
-        <f t="shared" ref="H31:H63" si="4">C31/E31</f>
+      <c r="G31" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B31,$K$3,$K$2,C31,D31,$K$2,E31,$K$2,F31,"),")</f>
+        <v>new Upgrade("Kylo Ren's Helmet",200000,1350,1),</v>
+      </c>
+      <c r="H31" s="12">
+        <f>C31/E31</f>
         <v>148.14814814814815</v>
       </c>
       <c r="I31" s="6">
-        <f t="shared" ref="I31:I63" si="5">FLOOR(LOG10(C31),1)</f>
-        <v>5</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N31" s="4"/>
     </row>
     <row r="32" spans="2:14">
       <c r="B32" s="1" t="s">
@@ -3731,20 +3838,21 @@
       <c r="F32" s="2">
         <v>5</v>
       </c>
-      <c r="G32" t="e">
-        <f>IF(A32="",_xlfn.CONCAT($K$1,#REF!,B32,#REF!,$K$2,C32,D32,$K$2,E32,$K$2,F32,"),",),_xlfn.CONCAT($K$1,#REF!,A32,#REF!,$K$2,#REF!,B32,#REF!,$K$2,C32,D32,$K$2,E32,$K$2,F32,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H32" s="12">
-        <f t="shared" si="4"/>
+      <c r="G32" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B32,$K$3,$K$2,C32,D32,$K$2,E32,$K$2,F32,"),")</f>
+        <v>new Upgrade("Nuclear Bomb",500235,2390,5),</v>
+      </c>
+      <c r="H32" s="11">
+        <f>C32/E32</f>
         <v>209.30334728033472</v>
       </c>
       <c r="I32">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N32" s="4"/>
+    </row>
+    <row r="33" spans="1:14">
       <c r="B33" s="1" t="s">
         <v>19</v>
       </c>
@@ -3761,20 +3869,21 @@
       <c r="F33" s="2">
         <v>10</v>
       </c>
-      <c r="G33" t="e">
-        <f>IF(A33="",_xlfn.CONCAT($K$1,#REF!,B33,#REF!,$K$2,C33,D33,$K$2,E33,$K$2,F33,"),",),_xlfn.CONCAT($K$1,#REF!,A33,#REF!,$K$2,#REF!,B33,#REF!,$K$2,C33,D33,$K$2,E33,$K$2,F33,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H33" s="12">
-        <f t="shared" si="4"/>
+      <c r="G33" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B33,$K$3,$K$2,C33,D33,$K$2,E33,$K$2,F33,"),")</f>
+        <v>new Upgrade("Bowcaster",155893,563,10),</v>
+      </c>
+      <c r="H33" s="11">
+        <f>C33/E33</f>
         <v>276.89698046181172</v>
       </c>
       <c r="I33">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" s="6" customFormat="1">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N33" s="4"/>
+    </row>
+    <row r="34" spans="1:14" s="6" customFormat="1">
       <c r="B34" s="7" t="s">
         <v>28</v>
       </c>
@@ -3792,23 +3901,24 @@
       <c r="F34" s="9">
         <v>1</v>
       </c>
-      <c r="G34" s="6" t="e">
-        <f>IF(A34="",_xlfn.CONCAT($K$1,#REF!,B34,#REF!,$K$2,C34,D34,$K$2,E34,$K$2,F34,"),",),_xlfn.CONCAT($K$1,#REF!,A34,#REF!,$K$2,#REF!,B34,#REF!,$K$2,C34,D34,$K$2,E34,$K$2,F34,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H34" s="13">
-        <f t="shared" si="4"/>
+      <c r="G34" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B34,$K$3,$K$2,C34,D34,$K$2,E34,$K$2,F34,"),")</f>
+        <v>new Upgrade("Genesis Device",765482,4570,1),</v>
+      </c>
+      <c r="H34" s="12">
+        <f>C34/E34</f>
         <v>167.50153172866521</v>
       </c>
       <c r="I34" s="6">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <f t="shared" ref="I34:I65" si="4">CEILING(LOG10(C34),1)</f>
+        <v>6</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
+        <v>95</v>
+      </c>
+      <c r="N34" s="4"/>
+    </row>
+    <row r="35" spans="1:14">
       <c r="B35" s="1" t="s">
         <v>42</v>
       </c>
@@ -3825,20 +3935,21 @@
       <c r="F35" s="2">
         <v>1</v>
       </c>
-      <c r="G35" t="e">
-        <f>IF(A35="",_xlfn.CONCAT($K$1,#REF!,B35,#REF!,$K$2,C35,D35,$K$2,E35,$K$2,F35,"),",),_xlfn.CONCAT($K$1,#REF!,A35,#REF!,$K$2,#REF!,B35,#REF!,$K$2,C35,D35,$K$2,E35,$K$2,F35,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H35" s="12">
+      <c r="G35" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B35,$K$3,$K$2,C35,D35,$K$2,E35,$K$2,F35,"),")</f>
+        <v>new Upgrade("A bad feeling about this",166830,1138,1),</v>
+      </c>
+      <c r="H35" s="11">
+        <f>C35/E35</f>
+        <v>146.59929701230229</v>
+      </c>
+      <c r="I35">
         <f t="shared" si="4"/>
-        <v>146.59929701230229</v>
-      </c>
-      <c r="I35">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" s="6" customFormat="1">
+        <v>6</v>
+      </c>
+      <c r="N35" s="4"/>
+    </row>
+    <row r="36" spans="1:14" s="6" customFormat="1">
       <c r="B36" s="7" t="s">
         <v>10</v>
       </c>
@@ -3855,23 +3966,24 @@
       <c r="F36" s="9">
         <v>2</v>
       </c>
-      <c r="G36" s="6" t="e">
-        <f>IF(A36="",_xlfn.CONCAT($K$1,#REF!,B36,#REF!,$K$2,C36,D36,$K$2,E36,$K$2,F36,"),",),_xlfn.CONCAT($K$1,#REF!,A36,#REF!,$K$2,#REF!,B36,#REF!,$K$2,C36,D36,$K$2,E36,$K$2,F36,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H36" s="13">
+      <c r="G36" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B36,$K$3,$K$2,C36,D36,$K$2,E36,$K$2,F36,"),")</f>
+        <v>new Upgrade("Death Star",1344339,7324,2),</v>
+      </c>
+      <c r="H36" s="12">
+        <f>C36/E36</f>
+        <v>183.55256690333152</v>
+      </c>
+      <c r="I36" s="6">
         <f t="shared" si="4"/>
-        <v>183.55256690333152</v>
-      </c>
-      <c r="I36" s="6">
-        <f t="shared" si="5"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
+        <v>95</v>
+      </c>
+      <c r="N36" s="4"/>
+    </row>
+    <row r="37" spans="1:14">
       <c r="B37" s="1" t="s">
         <v>6</v>
       </c>
@@ -3888,25 +4000,26 @@
       <c r="F37" s="2">
         <v>10</v>
       </c>
-      <c r="G37" t="e">
-        <f>IF(A37="",_xlfn.CONCAT($K$1,#REF!,B37,#REF!,$K$2,C37,D37,$K$2,E37,$K$2,F37,"),",),_xlfn.CONCAT($K$1,#REF!,A37,#REF!,$K$2,#REF!,B37,#REF!,$K$2,C37,D37,$K$2,E37,$K$2,F37,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H37" s="12">
+      <c r="G37" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B37,$K$3,$K$2,C37,D37,$K$2,E37,$K$2,F37,"),")</f>
+        <v>new Upgrade("Rocket",100000,500,10),</v>
+      </c>
+      <c r="H37" s="11">
+        <f>C37/E37</f>
+        <v>200</v>
+      </c>
+      <c r="I37">
         <f t="shared" si="4"/>
-        <v>200</v>
-      </c>
-      <c r="I37">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" s="6" customFormat="1">
+      <c r="N37" s="4"/>
+    </row>
+    <row r="38" spans="1:14" s="6" customFormat="1">
       <c r="A38" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C38" s="6">
         <v>2963500</v>
@@ -3922,23 +4035,24 @@
       <c r="F38" s="9">
         <v>19</v>
       </c>
-      <c r="G38" s="6" t="e">
-        <f>IF(A38="",_xlfn.CONCAT($K$1,#REF!,B38,#REF!,$K$2,C38,D38,$K$2,E38,$K$2,F38,"),",),_xlfn.CONCAT($K$1,#REF!,A38,#REF!,$K$2,#REF!,B38,#REF!,$K$2,C38,D38,$K$2,E38,$K$2,F38,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H38" s="13">
+      <c r="G38" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B38,$K$3,$K$2,C38,D38,$K$2,E38,$K$2,F38,"),")</f>
+        <v>new Upgrade("Ring of Power",2963500,19776,19),</v>
+      </c>
+      <c r="H38" s="12">
+        <f>C38/E38</f>
+        <v>149.85335760517799</v>
+      </c>
+      <c r="I38" s="6">
         <f t="shared" si="4"/>
-        <v>149.85335760517799</v>
-      </c>
-      <c r="I38" s="6">
-        <f t="shared" si="5"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" s="6" customFormat="1">
+        <v>95</v>
+      </c>
+      <c r="N38" s="4"/>
+    </row>
+    <row r="39" spans="1:14" s="6" customFormat="1">
       <c r="B39" s="7" t="s">
         <v>17</v>
       </c>
@@ -3955,23 +4069,24 @@
       <c r="F39" s="9">
         <v>1</v>
       </c>
-      <c r="G39" s="6" t="e">
-        <f>IF(A39="",_xlfn.CONCAT($K$1,#REF!,B39,#REF!,$K$2,C39,D39,$K$2,E39,$K$2,F39,"),",),_xlfn.CONCAT($K$1,#REF!,A39,#REF!,$K$2,#REF!,B39,#REF!,$K$2,C39,D39,$K$2,E39,$K$2,F39,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H39" s="13">
+      <c r="G39" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B39,$K$3,$K$2,C39,D39,$K$2,E39,$K$2,F39,"),")</f>
+        <v>new Upgrade("Stormbreaker",1375947,10000,1),</v>
+      </c>
+      <c r="H39" s="12">
+        <f>C39/E39</f>
+        <v>137.59469999999999</v>
+      </c>
+      <c r="I39" s="6">
         <f t="shared" si="4"/>
-        <v>137.59469999999999</v>
-      </c>
-      <c r="I39" s="6">
-        <f t="shared" si="5"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
+        <v>95</v>
+      </c>
+      <c r="N39" s="4"/>
+    </row>
+    <row r="40" spans="1:14">
       <c r="B40" s="1" t="s">
         <v>32</v>
       </c>
@@ -3988,22 +4103,23 @@
       <c r="F40" s="2">
         <v>10</v>
       </c>
-      <c r="G40" t="e">
-        <f>IF(A40="",_xlfn.CONCAT($K$1,#REF!,B40,#REF!,$K$2,C40,D40,$K$2,E40,$K$2,F40,"),",),_xlfn.CONCAT($K$1,#REF!,A40,#REF!,$K$2,#REF!,B40,#REF!,$K$2,C40,D40,$K$2,E40,$K$2,F40,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H40" s="12">
+      <c r="G40" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B40,$K$3,$K$2,C40,D40,$K$2,E40,$K$2,F40,"),")</f>
+        <v>new Upgrade("Medpack",100000,500,10),</v>
+      </c>
+      <c r="H40" s="11">
+        <f>C40/E40</f>
+        <v>200</v>
+      </c>
+      <c r="I40">
         <f t="shared" si="4"/>
-        <v>200</v>
-      </c>
-      <c r="I40">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" s="6" customFormat="1">
+      <c r="N40" s="4"/>
+    </row>
+    <row r="41" spans="1:14" s="6" customFormat="1">
       <c r="B41" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C41" s="6">
         <v>1019358</v>
@@ -4018,23 +4134,24 @@
       <c r="F41" s="9">
         <v>1</v>
       </c>
-      <c r="G41" s="6" t="e">
-        <f>IF(A41="",_xlfn.CONCAT($K$1,#REF!,B41,#REF!,$K$2,C41,D41,$K$2,E41,$K$2,F41,"),",),_xlfn.CONCAT($K$1,#REF!,A41,#REF!,$K$2,#REF!,B41,#REF!,$K$2,C41,D41,$K$2,E41,$K$2,F41,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H41" s="13">
+      <c r="G41" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B41,$K$3,$K$2,C41,D41,$K$2,E41,$K$2,F41,"),")</f>
+        <v>new Upgrade("Mario's Hat",1019358,5342,1),</v>
+      </c>
+      <c r="H41" s="12">
+        <f>C41/E41</f>
+        <v>190.81954324223136</v>
+      </c>
+      <c r="I41" s="6">
         <f t="shared" si="4"/>
-        <v>190.81954324223136</v>
-      </c>
-      <c r="I41" s="6">
-        <f t="shared" si="5"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
+        <v>95</v>
+      </c>
+      <c r="N41" s="4"/>
+    </row>
+    <row r="42" spans="1:14">
       <c r="B42" s="1" t="s">
         <v>44</v>
       </c>
@@ -4051,20 +4168,21 @@
       <c r="F42" s="2">
         <v>10</v>
       </c>
-      <c r="G42" t="e">
-        <f>IF(A42="",_xlfn.CONCAT($K$1,#REF!,B42,#REF!,$K$2,C42,D42,$K$2,E42,$K$2,F42,"),",),_xlfn.CONCAT($K$1,#REF!,A42,#REF!,$K$2,#REF!,B42,#REF!,$K$2,C42,D42,$K$2,E42,$K$2,F42,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H42" s="12">
+      <c r="G42" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B42,$K$3,$K$2,C42,D42,$K$2,E42,$K$2,F42,"),")</f>
+        <v>new Upgrade("Blender (the program)",530000,2140,10),</v>
+      </c>
+      <c r="H42" s="11">
+        <f>C42/E42</f>
+        <v>247.66355140186917</v>
+      </c>
+      <c r="I42">
         <f t="shared" si="4"/>
-        <v>247.66355140186917</v>
-      </c>
-      <c r="I42">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
+        <v>6</v>
+      </c>
+      <c r="N42" s="4"/>
+    </row>
+    <row r="43" spans="1:14">
       <c r="B43" s="1" t="s">
         <v>45</v>
       </c>
@@ -4081,23 +4199,24 @@
       <c r="F43" s="2">
         <v>1</v>
       </c>
-      <c r="G43" t="e">
-        <f>IF(A43="",_xlfn.CONCAT($K$1,#REF!,B43,#REF!,$K$2,C43,D43,$K$2,E43,$K$2,F43,"),",),_xlfn.CONCAT($K$1,#REF!,A43,#REF!,$K$2,#REF!,B43,#REF!,$K$2,C43,D43,$K$2,E43,$K$2,F43,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H43" s="12">
+      <c r="G43" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B43,$K$3,$K$2,C43,D43,$K$2,E43,$K$2,F43,"),")</f>
+        <v>new Upgrade("iPhone XR",300000,1215,1),</v>
+      </c>
+      <c r="H43" s="11">
+        <f>C43/E43</f>
+        <v>246.91358024691357</v>
+      </c>
+      <c r="I43">
         <f t="shared" si="4"/>
-        <v>246.91358024691357</v>
-      </c>
-      <c r="I43">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J43" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10">
+        <v>95</v>
+      </c>
+      <c r="N43" s="4"/>
+    </row>
+    <row r="44" spans="1:14">
       <c r="B44" s="1" t="s">
         <v>46</v>
       </c>
@@ -4114,23 +4233,24 @@
       <c r="F44" s="2">
         <v>10</v>
       </c>
-      <c r="G44" t="e">
-        <f>IF(A44="",_xlfn.CONCAT($K$1,#REF!,B44,#REF!,$K$2,C44,D44,$K$2,E44,$K$2,F44,"),",),_xlfn.CONCAT($K$1,#REF!,A44,#REF!,$K$2,#REF!,B44,#REF!,$K$2,C44,D44,$K$2,E44,$K$2,F44,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H44" s="12">
+      <c r="G44" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B44,$K$3,$K$2,C44,D44,$K$2,E44,$K$2,F44,"),")</f>
+        <v>new Upgrade("Stormtrooper Helmet",13630,70,10),</v>
+      </c>
+      <c r="H44" s="11">
+        <f>C44/E44</f>
+        <v>194.71428571428572</v>
+      </c>
+      <c r="I44">
         <f t="shared" si="4"/>
-        <v>194.71428571428572</v>
-      </c>
-      <c r="I44">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J44" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
+        <v>95</v>
+      </c>
+      <c r="N44" s="4"/>
+    </row>
+    <row r="45" spans="1:14">
       <c r="B45" s="1" t="s">
         <v>33</v>
       </c>
@@ -4147,23 +4267,24 @@
       <c r="F45" s="2">
         <v>10</v>
       </c>
-      <c r="G45" t="e">
-        <f>IF(A45="",_xlfn.CONCAT($K$1,#REF!,B45,#REF!,$K$2,C45,D45,$K$2,E45,$K$2,F45,"),",),_xlfn.CONCAT($K$1,#REF!,A45,#REF!,$K$2,#REF!,B45,#REF!,$K$2,C45,D45,$K$2,E45,$K$2,F45,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H45" s="12">
+      <c r="G45" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B45,$K$3,$K$2,C45,D45,$K$2,E45,$K$2,F45,"),")</f>
+        <v>new Upgrade("Sandwitch",22414,84,10),</v>
+      </c>
+      <c r="H45" s="11">
+        <f>C45/E45</f>
+        <v>266.83333333333331</v>
+      </c>
+      <c r="I45">
         <f t="shared" si="4"/>
-        <v>266.83333333333331</v>
-      </c>
-      <c r="I45">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J45" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
+        <v>95</v>
+      </c>
+      <c r="N45" s="4"/>
+    </row>
+    <row r="46" spans="1:14">
       <c r="B46" s="1" t="s">
         <v>65</v>
       </c>
@@ -4180,20 +4301,21 @@
       <c r="F46" s="2">
         <v>10</v>
       </c>
-      <c r="G46" t="e">
-        <f>IF(A46="",_xlfn.CONCAT($K$1,#REF!,B46,#REF!,$K$2,C46,D46,$K$2,E46,$K$2,F46,"),",),_xlfn.CONCAT($K$1,#REF!,A46,#REF!,$K$2,#REF!,B46,#REF!,$K$2,C46,D46,$K$2,E46,$K$2,F46,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H46" s="12">
+      <c r="G46" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B46,$K$3,$K$2,C46,D46,$K$2,E46,$K$2,F46,"),")</f>
+        <v>new Upgrade("Oculus",39999,199,10),</v>
+      </c>
+      <c r="H46" s="11">
+        <f>C46/E46</f>
+        <v>201</v>
+      </c>
+      <c r="I46">
         <f t="shared" si="4"/>
-        <v>201</v>
-      </c>
-      <c r="I46">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
+        <v>5</v>
+      </c>
+      <c r="N46" s="4"/>
+    </row>
+    <row r="47" spans="1:14">
       <c r="B47" s="1" t="s">
         <v>27</v>
       </c>
@@ -4210,20 +4332,21 @@
       <c r="F47" s="2">
         <v>6</v>
       </c>
-      <c r="G47" t="e">
-        <f>IF(A47="",_xlfn.CONCAT($K$1,#REF!,B47,#REF!,$K$2,C47,D47,$K$2,E47,$K$2,F47,"),",),_xlfn.CONCAT($K$1,#REF!,A47,#REF!,$K$2,#REF!,B47,#REF!,$K$2,C47,D47,$K$2,E47,$K$2,F47,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H47" s="12">
+      <c r="G47" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B47,$K$3,$K$2,C47,D47,$K$2,E47,$K$2,F47,"),")</f>
+        <v>new Upgrade("Shards of Narsil",20000,97,6),</v>
+      </c>
+      <c r="H47" s="11">
+        <f>C47/E47</f>
+        <v>206.18556701030928</v>
+      </c>
+      <c r="I47">
         <f t="shared" si="4"/>
-        <v>206.18556701030928</v>
-      </c>
-      <c r="I47">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
+        <v>5</v>
+      </c>
+      <c r="N47" s="4"/>
+    </row>
+    <row r="48" spans="1:14">
       <c r="B48" s="1" t="s">
         <v>5</v>
       </c>
@@ -4241,23 +4364,24 @@
       <c r="F48" s="2">
         <v>10</v>
       </c>
-      <c r="G48" t="e">
-        <f>IF(A48="",_xlfn.CONCAT($K$1,#REF!,B48,#REF!,$K$2,C48,D48,$K$2,E48,$K$2,F48,"),",),_xlfn.CONCAT($K$1,#REF!,A48,#REF!,$K$2,#REF!,B48,#REF!,$K$2,C48,D48,$K$2,E48,$K$2,F48,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H48" s="12">
+      <c r="G48" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B48,$K$3,$K$2,C48,D48,$K$2,E48,$K$2,F48,"),")</f>
+        <v>new Upgrade("Batarang",14645,70,10),</v>
+      </c>
+      <c r="H48" s="11">
+        <f>C48/E48</f>
+        <v>209.21428571428572</v>
+      </c>
+      <c r="I48">
         <f t="shared" si="4"/>
-        <v>209.21428571428572</v>
-      </c>
-      <c r="I48">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J48" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
+        <v>95</v>
+      </c>
+      <c r="N48" s="4"/>
+    </row>
+    <row r="49" spans="1:14">
       <c r="B49" s="1" t="s">
         <v>14</v>
       </c>
@@ -4274,20 +4398,21 @@
       <c r="F49" s="2">
         <v>100</v>
       </c>
-      <c r="G49" t="e">
-        <f>IF(A49="",_xlfn.CONCAT($K$1,#REF!,B49,#REF!,$K$2,C49,D49,$K$2,E49,$K$2,F49,"),",),_xlfn.CONCAT($K$1,#REF!,A49,#REF!,$K$2,#REF!,B49,#REF!,$K$2,C49,D49,$K$2,E49,$K$2,F49,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H49" s="12">
+      <c r="G49" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B49,$K$3,$K$2,C49,D49,$K$2,E49,$K$2,F49,"),")</f>
+        <v>new Upgrade("Sword",10000,51,100),</v>
+      </c>
+      <c r="H49" s="11">
+        <f>C49/E49</f>
+        <v>196.07843137254903</v>
+      </c>
+      <c r="I49">
         <f t="shared" si="4"/>
-        <v>196.07843137254903</v>
-      </c>
-      <c r="I49">
-        <f t="shared" si="5"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:10">
+      <c r="N49" s="4"/>
+    </row>
+    <row r="50" spans="1:14">
       <c r="B50" s="1" t="s">
         <v>34</v>
       </c>
@@ -4304,20 +4429,21 @@
       <c r="F50" s="2">
         <v>10</v>
       </c>
-      <c r="G50" t="e">
-        <f>IF(A50="",_xlfn.CONCAT($K$1,#REF!,B50,#REF!,$K$2,C50,D50,$K$2,E50,$K$2,F50,"),",),_xlfn.CONCAT($K$1,#REF!,A50,#REF!,$K$2,#REF!,B50,#REF!,$K$2,C50,D50,$K$2,E50,$K$2,F50,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H50" s="12">
+      <c r="G50" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B50,$K$3,$K$2,C50,D50,$K$2,E50,$K$2,F50,"),")</f>
+        <v>new Upgrade("Water Bottle",10000,49,10),</v>
+      </c>
+      <c r="H50" s="11">
+        <f>C50/E50</f>
+        <v>204.08163265306123</v>
+      </c>
+      <c r="I50">
         <f t="shared" si="4"/>
-        <v>204.08163265306123</v>
-      </c>
-      <c r="I50">
-        <f t="shared" si="5"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:10">
+      <c r="N50" s="4"/>
+    </row>
+    <row r="51" spans="1:14">
       <c r="B51" s="1" t="s">
         <v>39</v>
       </c>
@@ -4334,23 +4460,24 @@
       <c r="F51" s="2">
         <v>10</v>
       </c>
-      <c r="G51" t="e">
-        <f>IF(A51="",_xlfn.CONCAT($K$1,#REF!,B51,#REF!,$K$2,C51,D51,$K$2,E51,$K$2,F51,"),",),_xlfn.CONCAT($K$1,#REF!,A51,#REF!,$K$2,#REF!,B51,#REF!,$K$2,C51,D51,$K$2,E51,$K$2,F51,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H51" s="12">
+      <c r="G51" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B51,$K$3,$K$2,C51,D51,$K$2,E51,$K$2,F51,"),")</f>
+        <v>new Upgrade("Easy Button",667186,2839,10),</v>
+      </c>
+      <c r="H51" s="11">
+        <f>C51/E51</f>
+        <v>235.00739697076435</v>
+      </c>
+      <c r="I51">
         <f t="shared" si="4"/>
-        <v>235.00739697076435</v>
-      </c>
-      <c r="I51">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J51" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10">
+        <v>96</v>
+      </c>
+      <c r="N51" s="4"/>
+    </row>
+    <row r="52" spans="1:14">
       <c r="B52" s="1" t="s">
         <v>43</v>
       </c>
@@ -4367,20 +4494,21 @@
       <c r="F52" s="2">
         <v>7</v>
       </c>
-      <c r="G52" t="e">
-        <f>IF(A52="",_xlfn.CONCAT($K$1,#REF!,B52,#REF!,$K$2,C52,D52,$K$2,E52,$K$2,F52,"),",),_xlfn.CONCAT($K$1,#REF!,A52,#REF!,$K$2,#REF!,B52,#REF!,$K$2,C52,D52,$K$2,E52,$K$2,F52,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H52" s="12">
+      <c r="G52" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B52,$K$3,$K$2,C52,D52,$K$2,E52,$K$2,F52,"),")</f>
+        <v>new Upgrade("Blender (for food)",10000,43,7),</v>
+      </c>
+      <c r="H52" s="11">
+        <f>C52/E52</f>
+        <v>232.55813953488371</v>
+      </c>
+      <c r="I52">
         <f t="shared" si="4"/>
-        <v>232.55813953488371</v>
-      </c>
-      <c r="I52">
-        <f t="shared" si="5"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:10">
+      <c r="N52" s="4"/>
+    </row>
+    <row r="53" spans="1:14">
       <c r="B53" s="1" t="s">
         <v>64</v>
       </c>
@@ -4398,23 +4526,24 @@
       <c r="F53" s="2">
         <v>1</v>
       </c>
-      <c r="G53" t="e">
-        <f>IF(A53="",_xlfn.CONCAT($K$1,#REF!,B53,#REF!,$K$2,C53,D53,$K$2,E53,$K$2,F53,"),",),_xlfn.CONCAT($K$1,#REF!,A53,#REF!,$K$2,#REF!,B53,#REF!,$K$2,C53,D53,$K$2,E53,$K$2,F53,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H53" s="12">
+      <c r="G53" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B53,$K$3,$K$2,C53,D53,$K$2,E53,$K$2,F53,"),")</f>
+        <v>new Upgrade("The Piece of Resistance",998520,4950,1),</v>
+      </c>
+      <c r="H53" s="11">
+        <f>C53/E53</f>
+        <v>201.72121212121212</v>
+      </c>
+      <c r="I53">
         <f t="shared" si="4"/>
-        <v>201.72121212121212</v>
-      </c>
-      <c r="I53">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J53" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10">
+        <v>96</v>
+      </c>
+      <c r="N53" s="4"/>
+    </row>
+    <row r="54" spans="1:14">
       <c r="B54" s="1" t="s">
         <v>36</v>
       </c>
@@ -4431,20 +4560,21 @@
       <c r="F54" s="2">
         <v>200</v>
       </c>
-      <c r="G54" t="e">
-        <f>IF(A54="",_xlfn.CONCAT($K$1,#REF!,B54,#REF!,$K$2,C54,D54,$K$2,E54,$K$2,F54,"),",),_xlfn.CONCAT($K$1,#REF!,A54,#REF!,$K$2,#REF!,B54,#REF!,$K$2,C54,D54,$K$2,E54,$K$2,F54,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H54" s="12">
+      <c r="G54" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B54,$K$3,$K$2,C54,D54,$K$2,E54,$K$2,F54,"),")</f>
+        <v>new Upgrade("Shield",5000,25,200),</v>
+      </c>
+      <c r="H54" s="11">
+        <f>C54/E54</f>
+        <v>200</v>
+      </c>
+      <c r="I54">
         <f t="shared" si="4"/>
-        <v>200</v>
-      </c>
-      <c r="I54">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
+        <v>4</v>
+      </c>
+      <c r="N54" s="4"/>
+    </row>
+    <row r="55" spans="1:14">
       <c r="B55" s="1" t="s">
         <v>18</v>
       </c>
@@ -4461,22 +4591,23 @@
       <c r="F55" s="2">
         <v>4</v>
       </c>
-      <c r="G55" t="e">
-        <f>IF(A55="",_xlfn.CONCAT($K$1,#REF!,B55,#REF!,$K$2,C55,D55,$K$2,E55,$K$2,F55,"),",),_xlfn.CONCAT($K$1,#REF!,A55,#REF!,$K$2,#REF!,B55,#REF!,$K$2,C55,D55,$K$2,E55,$K$2,F55,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H55" s="12">
+      <c r="G55" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B55,$K$3,$K$2,C55,D55,$K$2,E55,$K$2,F55,"),")</f>
+        <v>new Upgrade("Shark Repellent Bat Spray",1996,10,4),</v>
+      </c>
+      <c r="H55" s="11">
+        <f>C55/E55</f>
+        <v>199.6</v>
+      </c>
+      <c r="I55">
         <f t="shared" si="4"/>
-        <v>199.6</v>
-      </c>
-      <c r="I55">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" s="6" customFormat="1">
+        <v>4</v>
+      </c>
+      <c r="N55" s="4"/>
+    </row>
+    <row r="56" spans="1:14" s="6" customFormat="1">
       <c r="B56" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C56" s="6">
         <v>957440</v>
@@ -4491,23 +4622,24 @@
       <c r="F56" s="9">
         <v>1</v>
       </c>
-      <c r="G56" s="6" t="e">
-        <f>IF(A56="",_xlfn.CONCAT($K$1,#REF!,B56,#REF!,$K$2,C56,D56,$K$2,E56,$K$2,F56,"),",),_xlfn.CONCAT($K$1,#REF!,A56,#REF!,$K$2,#REF!,B56,#REF!,$K$2,C56,D56,$K$2,E56,$K$2,F56,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H56" s="13">
+      <c r="G56" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B56,$K$3,$K$2,C56,D56,$K$2,E56,$K$2,F56,"),")</f>
+        <v>new Upgrade("Kirk's Glasses",957440,4329,1),</v>
+      </c>
+      <c r="H56" s="12">
+        <f>C56/E56</f>
+        <v>221.16886116886116</v>
+      </c>
+      <c r="I56" s="6">
         <f t="shared" si="4"/>
-        <v>221.16886116886116</v>
-      </c>
-      <c r="I56" s="6">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J56" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10">
+        <v>95</v>
+      </c>
+      <c r="N56" s="4"/>
+    </row>
+    <row r="57" spans="1:14">
       <c r="B57" s="1" t="s">
         <v>37</v>
       </c>
@@ -4524,20 +4656,21 @@
       <c r="F57" s="2">
         <v>100</v>
       </c>
-      <c r="G57" t="e">
-        <f>IF(A57="",_xlfn.CONCAT($K$1,#REF!,B57,#REF!,$K$2,C57,D57,$K$2,E57,$K$2,F57,"),",),_xlfn.CONCAT($K$1,#REF!,A57,#REF!,$K$2,#REF!,B57,#REF!,$K$2,C57,D57,$K$2,E57,$K$2,F57,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H57" s="12">
+      <c r="G57" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B57,$K$3,$K$2,C57,D57,$K$2,E57,$K$2,F57,"),")</f>
+        <v>new Upgrade("Popcorn",1000,5,100),</v>
+      </c>
+      <c r="H57" s="11">
+        <f>C57/E57</f>
+        <v>200</v>
+      </c>
+      <c r="I57">
         <f t="shared" si="4"/>
-        <v>200</v>
-      </c>
-      <c r="I57">
-        <f t="shared" si="5"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:10">
+      <c r="N57" s="4"/>
+    </row>
+    <row r="58" spans="1:14">
       <c r="B58" s="1" t="s">
         <v>63</v>
       </c>
@@ -4554,25 +4687,26 @@
       <c r="F58" s="2">
         <v>10</v>
       </c>
-      <c r="G58" t="e">
-        <f>IF(A58="",_xlfn.CONCAT($K$1,#REF!,B58,#REF!,$K$2,C58,D58,$K$2,E58,$K$2,F58,"),",),_xlfn.CONCAT($K$1,#REF!,A58,#REF!,$K$2,#REF!,B58,#REF!,$K$2,C58,D58,$K$2,E58,$K$2,F58,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H58" s="12">
+      <c r="G58" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B58,$K$3,$K$2,C58,D58,$K$2,E58,$K$2,F58,"),")</f>
+        <v>new Upgrade("Book",451,2,10),</v>
+      </c>
+      <c r="H58" s="11">
+        <f>C58/E58</f>
+        <v>225.5</v>
+      </c>
+      <c r="I58">
         <f t="shared" si="4"/>
-        <v>225.5</v>
-      </c>
-      <c r="I58">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10">
+        <v>3</v>
+      </c>
+      <c r="N58" s="4"/>
+    </row>
+    <row r="59" spans="1:14">
       <c r="A59" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B59" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C59">
         <v>100</v>
@@ -4587,20 +4721,21 @@
       <c r="F59" s="2">
         <v>1</v>
       </c>
-      <c r="G59" t="e">
-        <f>IF(A59="",_xlfn.CONCAT($K$1,#REF!,B59,#REF!,$K$2,C59,D59,$K$2,E59,$K$2,F59,"),",),_xlfn.CONCAT($K$1,#REF!,A59,#REF!,$K$2,#REF!,B59,#REF!,$K$2,C59,D59,$K$2,E59,$K$2,F59,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H59" s="12">
+      <c r="G59" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B59,$K$3,$K$2,C59,D59,$K$2,E59,$K$2,F59,"),")</f>
+        <v>new Upgrade("Cookie",100,3,1),</v>
+      </c>
+      <c r="H59" s="11">
+        <f>C59/E59</f>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="I59">
         <f t="shared" si="4"/>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="I59">
-        <f t="shared" si="5"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:10">
+      <c r="N59" s="4"/>
+    </row>
+    <row r="60" spans="1:14">
       <c r="B60" s="1" t="s">
         <v>31</v>
       </c>
@@ -4608,7 +4743,7 @@
         <v>200</v>
       </c>
       <c r="D60" t="str">
-        <f t="shared" ref="D60:D63" si="6">IF(C60&gt;2147483647,"L","")</f>
+        <f t="shared" ref="D60:D80" si="5">IF(C60&gt;2147483647,"L","")</f>
         <v/>
       </c>
       <c r="E60">
@@ -4617,20 +4752,21 @@
       <c r="F60" s="2">
         <v>100</v>
       </c>
-      <c r="G60" t="e">
-        <f>IF(A60="",_xlfn.CONCAT($K$1,#REF!,B60,#REF!,$K$2,C60,D60,$K$2,E60,$K$2,F60,"),",),_xlfn.CONCAT($K$1,#REF!,A60,#REF!,$K$2,#REF!,B60,#REF!,$K$2,C60,D60,$K$2,E60,$K$2,F60,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H60" s="12">
+      <c r="G60" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B60,$K$3,$K$2,C60,D60,$K$2,E60,$K$2,F60,"),")</f>
+        <v>new Upgrade("Lego Brick",200,1,100),</v>
+      </c>
+      <c r="H60" s="11">
+        <f>C60/E60</f>
+        <v>200</v>
+      </c>
+      <c r="I60">
         <f t="shared" si="4"/>
-        <v>200</v>
-      </c>
-      <c r="I60">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10">
+        <v>3</v>
+      </c>
+      <c r="N60" s="4"/>
+    </row>
+    <row r="61" spans="1:14">
       <c r="B61" s="1" t="s">
         <v>26</v>
       </c>
@@ -4638,7 +4774,7 @@
         <v>1</v>
       </c>
       <c r="D61" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="E61">
@@ -4647,83 +4783,709 @@
       <c r="F61" s="2">
         <v>128</v>
       </c>
-      <c r="G61" t="e">
-        <f>IF(A61="",_xlfn.CONCAT($K$1,#REF!,B61,#REF!,$K$2,C61,D61,$K$2,E61,$K$2,F61,"),",),_xlfn.CONCAT($K$1,#REF!,A61,#REF!,$K$2,#REF!,B61,#REF!,$K$2,C61,D61,$K$2,E61,$K$2,F61,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H61" s="12">
-        <f t="shared" si="4"/>
+      <c r="G61" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B61,$K$3,$K$2,C61,D61,$K$2,E61,$K$2,F61,"),")</f>
+        <v>new Upgrade("Bug",1,-1,128),</v>
+      </c>
+      <c r="H61" s="11">
+        <f>C61/E61</f>
         <v>-1</v>
       </c>
       <c r="I61">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10">
-      <c r="A62" t="s">
-        <v>100</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="N61" s="4"/>
+    </row>
+    <row r="62" spans="1:14">
       <c r="B62" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>59637044043</v>
       </c>
       <c r="D62" t="str">
-        <f>IF(C62&gt;2147483647,"L","")</f>
-        <v/>
+        <f t="shared" si="5"/>
+        <v>L</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <f>MROUND(Table1[[#This Row],[Cost]]/Table1[[#This Row],[Messages needed to earn back the amount of coins spend]],1)</f>
+        <v>141467051</v>
       </c>
       <c r="F62" s="2">
         <v>1</v>
       </c>
-      <c r="G62" t="str">
-        <f>IF(A62="",_xlfn.CONCAT($K$1,$K$2,B62,$K$2,$K$3,C62,D62,$K$3,E62,$K$3,F62,"),",),_xlfn.CONCAT($K$1,$K$2,A62,$K$2,$K$3,$K$2,B62,$K$2,$K$3,C62,D62,$K$3,E62,$K$3,F62,"),"))</f>
-        <v>new Upgrade(,OP,,Cheat,111),</v>
-      </c>
-      <c r="H62" s="12">
-        <f>C62/E62</f>
-        <v>1</v>
+      <c r="G62" s="4" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B62,$K$3,$K$2,C62,D62,$K$2,E62,$K$2,F62,"),")</f>
+        <v>new Upgrade("Arc Reactor",59637044043L,141467051,1),</v>
+      </c>
+      <c r="H62" s="11">
+        <f t="shared" ref="H62:H64" si="6">16*LOG(C62,6)+200</f>
+        <v>421.56137082818816</v>
       </c>
       <c r="I62" s="4">
-        <f>FLOOR(LOG10(C62),1)</f>
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="J62" t="s">
+        <v>95</v>
+      </c>
+      <c r="M62" s="3"/>
+      <c r="N62" s="4"/>
+    </row>
+    <row r="63" spans="1:14">
+      <c r="B63" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C63">
+        <v>2110089696934650</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="5"/>
+        <v>L</v>
+      </c>
+      <c r="E63">
+        <f>MROUND(Table1[[#This Row],[Cost]]/Table1[[#This Row],[Messages needed to earn back the amount of coins spend]],1)</f>
+        <v>4096534023712</v>
+      </c>
+      <c r="F63" s="2">
+        <v>1</v>
+      </c>
+      <c r="G63" s="4" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B63,$K$3,$K$2,C63,D63,$K$2,E63,$K$2,F63,"),")</f>
+        <v>new Upgrade("Kryptonite",2110089696934650L,4096534023712,1),</v>
+      </c>
+      <c r="H63" s="11">
+        <f t="shared" si="6"/>
+        <v>515.09146139659265</v>
+      </c>
+      <c r="I63" s="4">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="J63" t="s">
+        <v>95</v>
+      </c>
+      <c r="N63" s="4"/>
+    </row>
+    <row r="64" spans="1:14">
+      <c r="B64" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C64">
+        <v>8.3250280290413904E+16</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="5"/>
+        <v>L</v>
+      </c>
+      <c r="E64">
+        <f>MROUND(Table1[[#This Row],[Cost]]/Table1[[#This Row],[Messages needed to earn back the amount of coins spend]],1)</f>
+        <v>151941677102307</v>
+      </c>
+      <c r="F64" s="2">
+        <v>1</v>
+      </c>
+      <c r="G64" s="4" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B64,$K$3,$K$2,C64,D64,$K$2,E64,$K$2,F64,"),")</f>
+        <v>new Upgrade("Air Force One",83250280290413900L,151941677102307,1),</v>
+      </c>
+      <c r="H64" s="11">
+        <f t="shared" si="6"/>
+        <v>547.90944708579946</v>
+      </c>
+      <c r="I64" s="4">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="J64" t="s">
+        <v>95</v>
+      </c>
+      <c r="N64" s="4"/>
+    </row>
+    <row r="65" spans="1:14">
+      <c r="A65" t="s">
+        <v>98</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65" s="2">
+        <v>1</v>
+      </c>
+      <c r="G65" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B65,$K$3,$K$2,C65,D65,$K$2,E65,$K$2,F65,"),")</f>
+        <v>new Upgrade("Cheat",1,1,1),</v>
+      </c>
+      <c r="H65" s="11">
+        <f>C65/E65</f>
+        <v>1</v>
+      </c>
+      <c r="I65" s="4">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:10">
-      <c r="B63" s="1" t="s">
+      <c r="N65" s="4"/>
+    </row>
+    <row r="66" spans="1:14">
+      <c r="B66" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C66">
+        <v>40896568606</v>
+      </c>
+      <c r="D66" t="str">
+        <f>IF(C66&gt;2147483647,"L","")</f>
+        <v>L</v>
+      </c>
+      <c r="E66">
+        <f>MROUND(Table1[[#This Row],[Cost]]/Table1[[#This Row],[Messages needed to earn back the amount of coins spend]],1)</f>
+        <v>97793577</v>
+      </c>
+      <c r="F66" s="2"/>
+      <c r="G66" s="4" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B66,$K$3,$K$2,C66,D66,$K$2,E66,$K$2,F66,"),")</f>
+        <v>new Upgrade("Ice Cream",40896568606L,97793577,),</v>
+      </c>
+      <c r="H66" s="11">
+        <f t="shared" ref="H66" si="7">16*LOG(C66,6)+200</f>
+        <v>418.19278686855296</v>
+      </c>
+      <c r="I66" s="4">
+        <f t="shared" ref="I66:I80" si="8">CEILING(LOG10(C66),1)</f>
+        <v>11</v>
+      </c>
+      <c r="N66" s="4"/>
+    </row>
+    <row r="67" spans="1:14">
+      <c r="B67" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C67">
+        <v>4.2751491899335398E+18</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" ref="D67:D70" si="9">IF(C67&gt;2147483647,"L","")</f>
+        <v>L</v>
+      </c>
+      <c r="E67">
+        <f>MROUND(Table1[[#This Row],[Cost]]/Table1[[#This Row],[Messages needed to earn back the amount of coins spend]],1)</f>
+        <v>7331994574249421</v>
+      </c>
+      <c r="F67" s="2">
+        <v>1</v>
+      </c>
+      <c r="G67" s="4" t="str">
+        <f t="shared" ref="G67:G70" si="10">_xlfn.CONCAT($K$1,$K$3,B67,$K$3,$K$2,C67,D67,$K$2,E67,$K$2,F67,"),")</f>
+        <v>new Upgrade("Klondike Bar",4275149189933540000L,7331994574249420,1),</v>
+      </c>
+      <c r="H67" s="11">
+        <f t="shared" ref="H67:H79" si="11">16*LOG(C67,6)+200</f>
+        <v>583.081335732056</v>
+      </c>
+      <c r="I67" s="4">
+        <f t="shared" si="8"/>
+        <v>19</v>
+      </c>
+      <c r="J67" t="s">
+        <v>95</v>
+      </c>
+      <c r="N67" s="4"/>
+    </row>
+    <row r="68" spans="1:14">
+      <c r="B68" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C68">
+        <v>83745097494464</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="9"/>
+        <v>L</v>
+      </c>
+      <c r="E68">
+        <f>MROUND(Table1[[#This Row],[Cost]]/Table1[[#This Row],[Messages needed to earn back the amount of coins spend]],1)</f>
+        <v>172216610960</v>
+      </c>
+      <c r="F68" s="2">
+        <v>1</v>
+      </c>
+      <c r="G68" s="4" t="str">
+        <f t="shared" si="10"/>
+        <v>new Upgrade("Time Machine",83745097494464L,172216610960,1),</v>
+      </c>
+      <c r="H68" s="11">
+        <f t="shared" si="11"/>
+        <v>486.27770008752549</v>
+      </c>
+      <c r="I68" s="4">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="J68" t="s">
+        <v>95</v>
+      </c>
+      <c r="N68" s="4"/>
+    </row>
+    <row r="69" spans="1:14">
+      <c r="B69" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C69">
+        <v>1000000</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69" s="2">
+        <v>1</v>
+      </c>
+      <c r="G69" s="4" t="str">
+        <f t="shared" si="10"/>
+        <v>new Upgrade("Bribe",1000000,0,1),</v>
+      </c>
+      <c r="H69" s="11">
+        <v>0</v>
+      </c>
+      <c r="I69" s="4">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="N69" s="4"/>
+    </row>
+    <row r="70" spans="1:14">
+      <c r="B70" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C70">
+        <v>81247450573750</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="9"/>
+        <v>L</v>
+      </c>
+      <c r="E70">
+        <f>MROUND(Table1[[#This Row],[Cost]]/Table1[[#This Row],[Messages needed to earn back the amount of coins spend]],1)</f>
+        <v>167173305334</v>
+      </c>
+      <c r="F70" s="2">
+        <v>1</v>
+      </c>
+      <c r="G70" s="4" t="str">
+        <f t="shared" si="10"/>
+        <v>new Upgrade("Nuclear Fireworks",81247450573750L,167173305334,1),</v>
+      </c>
+      <c r="H70" s="11">
+        <f t="shared" si="11"/>
+        <v>486.00732282791182</v>
+      </c>
+      <c r="I70" s="4">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="J70" t="s">
+        <v>95</v>
+      </c>
+      <c r="N70" s="4"/>
+    </row>
+    <row r="71" spans="1:14">
+      <c r="B71" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C71">
+        <v>1755841378694</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" ref="D71:D76" si="12">IF(C71&gt;2147483647,"L","")</f>
+        <v>L</v>
+      </c>
+      <c r="E71">
+        <f>MROUND(Table1[[#This Row],[Cost]]/Table1[[#This Row],[Messages needed to earn back the amount of coins spend]],1)</f>
+        <v>3886619829</v>
+      </c>
+      <c r="F71" s="2">
+        <v>1</v>
+      </c>
+      <c r="G71" s="4" t="str">
+        <f t="shared" ref="G71:G76" si="13">_xlfn.CONCAT($K$1,$K$3,B71,$K$3,$K$2,C71,D71,$K$2,E71,$K$2,F71,"),")</f>
+        <v>new Upgrade("Meme",1755841378694L,3886619829,1),</v>
+      </c>
+      <c r="H71" s="11">
+        <f t="shared" si="11"/>
+        <v>451.76566172171169</v>
+      </c>
+      <c r="I71" s="4">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="J71" t="s">
+        <v>95</v>
+      </c>
+      <c r="N71" s="4"/>
+    </row>
+    <row r="72" spans="1:14">
+      <c r="B72" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C72">
+        <v>79837291968785</v>
+      </c>
+      <c r="D72" t="str">
+        <f>IF(C72&gt;2147483647,"L","")</f>
+        <v>L</v>
+      </c>
+      <c r="E72">
+        <f>MROUND(Table1[[#This Row],[Cost]]/Table1[[#This Row],[Messages needed to earn back the amount of coins spend]],1)</f>
+        <v>164324651505</v>
+      </c>
+      <c r="F72" s="2">
+        <v>1</v>
+      </c>
+      <c r="G72" s="4" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B72,$K$3,$K$2,C72,D72,$K$2,E72,$K$2,F72,"),")</f>
+        <v>new Upgrade("Bigfoot",79837291968785L,164324651505,1),</v>
+      </c>
+      <c r="H72" s="11">
+        <f t="shared" si="11"/>
+        <v>485.85097389592102</v>
+      </c>
+      <c r="I72" s="4">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="J72" t="s">
+        <v>95</v>
+      </c>
+      <c r="N72" s="4"/>
+    </row>
+    <row r="73" spans="1:14">
+      <c r="B73" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C73">
+        <v>5704058330541</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" ref="D73:D75" si="14">IF(C73&gt;2147483647,"L","")</f>
+        <v>L</v>
+      </c>
+      <c r="E73">
+        <f>MROUND(Table1[[#This Row],[Cost]]/Table1[[#This Row],[Messages needed to earn back the amount of coins spend]],1)</f>
+        <v>12338782071</v>
+      </c>
+      <c r="F73" s="2">
+        <v>1</v>
+      </c>
+      <c r="G73" s="4" t="str">
+        <f t="shared" ref="G73:G75" si="15">_xlfn.CONCAT($K$1,$K$3,B73,$K$3,$K$2,C73,D73,$K$2,E73,$K$2,F73,"),")</f>
+        <v>new Upgrade("Area 51",5704058330541L,12338782071,1),</v>
+      </c>
+      <c r="H73" s="11">
+        <f t="shared" si="11"/>
+        <v>462.28698241863572</v>
+      </c>
+      <c r="I73" s="4">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="J73" t="s">
+        <v>95</v>
+      </c>
+      <c r="N73" s="4"/>
+    </row>
+    <row r="74" spans="1:14">
+      <c r="B74" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C74">
+        <v>2221819257185</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="14"/>
+        <v>L</v>
+      </c>
+      <c r="E74">
+        <f>MROUND(Table1[[#This Row],[Cost]]/Table1[[#This Row],[Messages needed to earn back the amount of coins spend]],1)</f>
+        <v>4895303336</v>
+      </c>
+      <c r="F74" s="2">
+        <v>1</v>
+      </c>
+      <c r="G74" s="4" t="str">
+        <f t="shared" si="15"/>
+        <v>new Upgrade("Loch Ness Monster",2221819257185L,4895303336,1),</v>
+      </c>
+      <c r="H74" s="11">
+        <f t="shared" si="11"/>
+        <v>453.86753478632716</v>
+      </c>
+      <c r="I74" s="4">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="J74" t="s">
+        <v>95</v>
+      </c>
+      <c r="N74" s="4"/>
+    </row>
+    <row r="75" spans="1:14">
+      <c r="B75" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C75">
+        <v>839548670437</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="14"/>
+        <v>L</v>
+      </c>
+      <c r="E75">
+        <f>MROUND(Table1[[#This Row],[Cost]]/Table1[[#This Row],[Messages needed to earn back the amount of coins spend]],1)</f>
+        <v>1885876413</v>
+      </c>
+      <c r="F75" s="2">
+        <v>1</v>
+      </c>
+      <c r="G75" s="4" t="str">
+        <f t="shared" si="15"/>
+        <v>new Upgrade("The Moon",839548670437L,1885876413,1),</v>
+      </c>
+      <c r="H75" s="11">
+        <f t="shared" si="11"/>
+        <v>445.17692923698598</v>
+      </c>
+      <c r="I75" s="4">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="J75" t="s">
+        <v>95</v>
+      </c>
+      <c r="N75" s="4"/>
+    </row>
+    <row r="76" spans="1:14">
+      <c r="B76" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C76">
+        <v>1248529473245030</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="12"/>
+        <v>L</v>
+      </c>
+      <c r="E76">
+        <f>MROUND(Table1[[#This Row],[Cost]]/Table1[[#This Row],[Messages needed to earn back the amount of coins spend]],1)</f>
+        <v>2446152366149</v>
+      </c>
+      <c r="F76" s="2">
+        <v>5</v>
+      </c>
+      <c r="G76" s="4" t="str">
+        <f t="shared" si="13"/>
+        <v>new Upgrade("A True Cake",1248529473245030L,2446152366149,5),</v>
+      </c>
+      <c r="H76" s="11">
+        <f t="shared" si="11"/>
+        <v>510.40543938429477</v>
+      </c>
+      <c r="I76" s="4">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="J76" t="s">
+        <v>95</v>
+      </c>
+      <c r="N76" s="4"/>
+    </row>
+    <row r="77" spans="1:14">
+      <c r="B77" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C77">
+        <v>55905021527</v>
+      </c>
+      <c r="D77" t="str">
+        <f>IF(C77&gt;2147483647,"L","")</f>
+        <v>L</v>
+      </c>
+      <c r="E77">
+        <f>MROUND(Table1[[#This Row],[Cost]]/Table1[[#This Row],[Messages needed to earn back the amount of coins spend]],1)</f>
+        <v>132795976</v>
+      </c>
+      <c r="F77" s="2">
+        <v>1</v>
+      </c>
+      <c r="G77" s="4" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B77,$K$3,$K$2,C77,D77,$K$2,E77,$K$2,F77,"),")</f>
+        <v>new Upgrade("MissingNo",55905021527L,132795976,1),</v>
+      </c>
+      <c r="H77" s="11">
+        <f t="shared" si="11"/>
+        <v>420.98430481204133</v>
+      </c>
+      <c r="I77" s="4">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+      <c r="J77" t="s">
+        <v>95</v>
+      </c>
+      <c r="N77" s="4"/>
+    </row>
+    <row r="78" spans="1:14">
+      <c r="B78" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C78">
+        <v>37910263806</v>
+      </c>
+      <c r="D78" t="str">
+        <f>IF(C78&gt;2147483647,"L","")</f>
+        <v>L</v>
+      </c>
+      <c r="E78">
+        <f>MROUND(Table1[[#This Row],[Cost]]/Table1[[#This Row],[Messages needed to earn back the amount of coins spend]],1)</f>
+        <v>90799614</v>
+      </c>
+      <c r="F78" s="2">
+        <v>2</v>
+      </c>
+      <c r="G78" s="4" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B78,$K$3,$K$2,C78,D78,$K$2,E78,$K$2,F78,"),")</f>
+        <v>new Upgrade("Airpods",37910263806L,90799614,2),</v>
+      </c>
+      <c r="H78" s="11">
+        <f t="shared" si="11"/>
+        <v>417.51569353838971</v>
+      </c>
+      <c r="I78" s="4">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+      <c r="J78" t="s">
+        <v>95</v>
+      </c>
+      <c r="N78" s="4"/>
+    </row>
+    <row r="79" spans="1:14">
+      <c r="B79" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C79">
+        <v>1858055186797720</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" ref="D79" si="16">IF(C79&gt;2147483647,"L","")</f>
+        <v>L</v>
+      </c>
+      <c r="E79">
+        <f>MROUND(Table1[[#This Row],[Cost]]/Table1[[#This Row],[Messages needed to earn back the amount of coins spend]],1)</f>
+        <v>3615205690620</v>
+      </c>
+      <c r="F79" s="2">
+        <v>2</v>
+      </c>
+      <c r="G79" s="4" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B79,$K$3,$K$2,C79,D79,$K$2,E79,$K$2,F79,"),")</f>
+        <v>new Upgrade("Iron Man Suit",1858055186797720L,3615205690620,2),</v>
+      </c>
+      <c r="H79" s="11">
+        <f t="shared" si="11"/>
+        <v>513.95559362456413</v>
+      </c>
+      <c r="I79" s="4">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="J79" t="s">
+        <v>95</v>
+      </c>
+      <c r="N79" s="4"/>
+    </row>
+    <row r="80" spans="1:14">
+      <c r="B80" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C63">
-        <v>1</v>
-      </c>
-      <c r="D63" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="E63">
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E80">
         <v>0</v>
       </c>
-      <c r="F63" s="2">
+      <c r="F80" s="2">
         <v>256</v>
       </c>
-      <c r="G63" t="e">
-        <f>IF(A63="",_xlfn.CONCAT($K$1,#REF!,B63,#REF!,$K$2,C63,D63,$K$2,E63,$K$2,F63,"),",),_xlfn.CONCAT($K$1,#REF!,A63,#REF!,$K$2,#REF!,B63,#REF!,$K$2,C63,D63,$K$2,E63,$K$2,F63,"),"))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H63" s="12" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I63">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="G80" t="str">
+        <f>_xlfn.CONCAT($K$1,$K$3,B80,$K$3,$K$2,C80,D80,$K$2,E80,$K$2,F80,"),")</f>
+        <v>new Upgrade("Debug Byte",1,0,256),</v>
+      </c>
+      <c r="H80" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="I80">
+        <v>1</v>
+      </c>
+      <c r="N80" s="4"/>
+    </row>
+    <row r="81" spans="14:14">
+      <c r="N81" s="4"/>
+    </row>
+    <row r="82" spans="14:14">
+      <c r="N82" s="4"/>
+    </row>
+    <row r="83" spans="14:14">
+      <c r="N83" s="4"/>
+    </row>
+    <row r="84" spans="14:14">
+      <c r="N84" s="4"/>
+    </row>
+    <row r="85" spans="14:14">
+      <c r="N85" s="4"/>
+    </row>
+    <row r="86" spans="14:14">
+      <c r="N86" s="4"/>
+    </row>
+    <row r="87" spans="14:14">
+      <c r="N87" s="4"/>
+    </row>
+    <row r="88" spans="14:14">
+      <c r="N88" s="4"/>
+    </row>
+    <row r="89" spans="14:14">
+      <c r="N89" s="4"/>
+    </row>
+    <row r="90" spans="14:14">
+      <c r="N90" s="4"/>
+    </row>
+    <row r="91" spans="14:14">
+      <c r="N91" s="4"/>
+    </row>
+    <row r="92" spans="14:14">
+      <c r="N92" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K5:L7"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>9223372036854770000</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>